<commit_message>
Update app.py with time series analysis application
</commit_message>
<xml_diff>
--- a/Variables Macroeconómicas.xlsx
+++ b/Variables Macroeconómicas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjacome\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjacome\Documents\DIPLOMADO MERCADO DE VALORES UNIVERSIDAD AZUAY\Presentaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854D43AA-E687-48E7-8E9F-92EBCC8A4081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314D2AB2-AE99-4662-853A-979E7BAFB890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{09660F72-473F-4D46-9A0D-D9BE093B6C6A}"/>
   </bookViews>
@@ -221,7 +221,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -557,10 +557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977AEE5-C7D7-4843-A708-BBC79C1628E8}">
-  <dimension ref="A1:AS70"/>
+  <dimension ref="A1:AS71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE34" workbookViewId="0">
-      <selection sqref="A1:AS70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10181,6 +10182,141 @@
         <v>114.81</v>
       </c>
     </row>
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>45931</v>
+      </c>
+      <c r="B71" s="2">
+        <v>21220.630369739982</v>
+      </c>
+      <c r="C71" s="2">
+        <v>108.914074</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2">
+        <v>11779.900349999989</v>
+      </c>
+      <c r="F71" s="2">
+        <v>33109.444793739967</v>
+      </c>
+      <c r="G71" s="2">
+        <v>64339.601249999905</v>
+      </c>
+      <c r="H71" s="2">
+        <v>97449.046043739872</v>
+      </c>
+      <c r="I71" s="2">
+        <v>5716.633992359999</v>
+      </c>
+      <c r="J71" s="2">
+        <v>490.87055126000001</v>
+      </c>
+      <c r="K71" s="2">
+        <v>1728.892597</v>
+      </c>
+      <c r="L71" s="2">
+        <v>29265.941584359978</v>
+      </c>
+      <c r="M71" s="2">
+        <v>1.1313302426406127</v>
+      </c>
+      <c r="N71" s="2">
+        <v>3.3297765514511122</v>
+      </c>
+      <c r="O71" s="2">
+        <v>15321.776446449991</v>
+      </c>
+      <c r="P71" s="2">
+        <v>1616.24894004</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>1962.9243429999999</v>
+      </c>
+      <c r="R71" s="2">
+        <v>7198.1963599999899</v>
+      </c>
+      <c r="S71" s="2">
+        <v>4544.4068034100001</v>
+      </c>
+      <c r="T71" s="2">
+        <v>64339.601317999899</v>
+      </c>
+      <c r="U71" s="2">
+        <v>132.88802799999999</v>
+      </c>
+      <c r="V71" s="2">
+        <v>11.716444000000001</v>
+      </c>
+      <c r="W71" s="2">
+        <v>9098.2015870000014</v>
+      </c>
+      <c r="X71" s="2">
+        <v>55096.795258999904</v>
+      </c>
+      <c r="Y71" s="2">
+        <v>73886.177232809991</v>
+      </c>
+      <c r="Z71" s="2">
+        <v>26062.745223000002</v>
+      </c>
+      <c r="AA71" s="2">
+        <v>42383.961760000006</v>
+      </c>
+      <c r="AB71" s="2">
+        <v>702.19220599999994</v>
+      </c>
+      <c r="AC71" s="2">
+        <v>3126.3338269999899</v>
+      </c>
+      <c r="AD71" s="2">
+        <v>1488.6902462999979</v>
+      </c>
+      <c r="AE71" s="2">
+        <v>122.25397051</v>
+      </c>
+      <c r="AF71" s="2">
+        <v>1847791155.2179408</v>
+      </c>
+      <c r="AG71" s="2">
+        <v>358235729.72144401</v>
+      </c>
+      <c r="AH71" s="2">
+        <v>273670999.82038802</v>
+      </c>
+      <c r="AI71" s="2">
+        <v>206601424.527722</v>
+      </c>
+      <c r="AJ71" s="2">
+        <v>376469310.882388</v>
+      </c>
+      <c r="AK71" s="2">
+        <v>149444110.876111</v>
+      </c>
+      <c r="AL71" s="2">
+        <v>9180099.0999999996</v>
+      </c>
+      <c r="AM71" s="2">
+        <v>223822486.08111101</v>
+      </c>
+      <c r="AN71" s="2">
+        <v>214553079.31999901</v>
+      </c>
+      <c r="AO71" s="2">
+        <v>262019.808111119</v>
+      </c>
+      <c r="AP71" s="2">
+        <v>27472049.450666599</v>
+      </c>
+      <c r="AQ71" s="2">
+        <v>8079845.6300000399</v>
+      </c>
+      <c r="AR71" s="2">
+        <v>4.2549999999999998E-2</v>
+      </c>
+      <c r="AS71" s="2">
+        <v>114.8071371148976</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>